<commit_message>
input file added, README modified correspondingly
</commit_message>
<xml_diff>
--- a/output/Attachment_1564702282.xlsx
+++ b/output/Attachment_1564702282.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\github_repos\work-8\output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="244" yWindow="11" windowWidth="16095" windowHeight="9659"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -144,8 +139,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,14 +203,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -262,7 +249,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -294,10 +281,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -329,7 +315,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -505,16 +490,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -582,7 +565,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22">
       <c r="A2">
         <v>1912</v>
       </c>
@@ -608,7 +591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22">
       <c r="A3">
         <v>2021</v>
       </c>
@@ -634,7 +617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22">
       <c r="A4">
         <v>2253</v>
       </c>
@@ -663,7 +646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22">
       <c r="A5">
         <v>2811</v>
       </c>

</xml_diff>